<commit_message>
deleted video info in excel, added stymuls right to the tasks in a list format
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\iONKiD\iONKiD_chatbot_testing-Mort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5551CB-D150-4BD5-BE11-4EF6EBBB651E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BD7388-8414-476A-B41E-9D8D6F3690E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{16AF0F94-C632-4BB3-8644-C0CDC664E6A8}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>VideoIsNecessary</t>
-  </si>
-  <si>
     <t>Text1</t>
   </si>
   <si>
@@ -63,15 +60,6 @@
     <t>мяч</t>
   </si>
   <si>
-    <t>так</t>
-  </si>
-  <si>
-    <t>ні</t>
-  </si>
-  <si>
-    <t>ябклуко</t>
-  </si>
-  <si>
     <t>пастила</t>
   </si>
   <si>
@@ -97,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">Показуйте картинки і розповідайте, що на них зображено в деталях. Показуйте на зображенні, про що саме ви говорите. Дитина повинна візуально сприймати інформацію, яку вона бачить перед собою, та стежити за рухом вашого пальця. Стежте за увагою дитини під час цієї вправи. </t>
+  </si>
+  <si>
+    <t>яблуко</t>
   </si>
 </sst>
 </file>
@@ -449,22 +440,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A589D644-B105-4A4C-9296-A1CC2137205D}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="141.5546875" customWidth="1"/>
-    <col min="4" max="4" width="190.44140625" customWidth="1"/>
-    <col min="5" max="5" width="206.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="141.5546875" customWidth="1"/>
+    <col min="3" max="3" width="190.44140625" customWidth="1"/>
+    <col min="4" max="4" width="206.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,16 +467,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -495,33 +482,30 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -530,30 +514,24 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>